<commit_message>
Week 6 update - inventory, ads, business, templates & ETL changes
</commit_message>
<xml_diff>
--- a/data/ams_weekly_data/Audio_Array/business_report_week5.xlsx
+++ b/data/ams_weekly_data/Audio_Array/business_report_week5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\raw\sales\Week 5\Audio_Array\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\ams_weekly_data\Audio_Array\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC89A353-6297-46FF-9190-88E3B6DA66CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB35E13D-A711-47CC-B133-EDDD38FC3807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92AC20E1-B4EA-4C08-82A7-BD2223CFA089}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="513">
   <si>
     <t>SKU</t>
   </si>
@@ -1561,6 +1561,15 @@
   </si>
   <si>
     <t>B0DFMLQBMC</t>
+  </si>
+  <si>
+    <t>FBA79844</t>
+  </si>
+  <si>
+    <t>PB-08 (AM-C1 + AI-04)</t>
+  </si>
+  <si>
+    <t>B0FN7DYB2M</t>
   </si>
 </sst>
 </file>
@@ -2407,15 +2416,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886434C-1F55-417D-A08D-842D1465F6AB}">
-  <dimension ref="A1:Y176"/>
+  <dimension ref="A1:Y251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S178" sqref="S178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="20" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15092,6 +15102,1506 @@
       </c>
       <c r="X176" s="3"/>
     </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>95</v>
+      </c>
+      <c r="B177" t="s">
+        <v>96</v>
+      </c>
+      <c r="C177" t="s">
+        <v>97</v>
+      </c>
+      <c r="D177" t="s">
+        <v>97</v>
+      </c>
+      <c r="P177">
+        <v>112</v>
+      </c>
+      <c r="T177" s="3">
+        <v>436515.52</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>226</v>
+      </c>
+      <c r="B178" t="s">
+        <v>227</v>
+      </c>
+      <c r="C178" t="s">
+        <v>228</v>
+      </c>
+      <c r="D178" t="s">
+        <v>228</v>
+      </c>
+      <c r="P178">
+        <v>184</v>
+      </c>
+      <c r="T178" s="3">
+        <v>420860.59</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>370</v>
+      </c>
+      <c r="B179" t="s">
+        <v>371</v>
+      </c>
+      <c r="C179" t="s">
+        <v>372</v>
+      </c>
+      <c r="D179" t="s">
+        <v>372</v>
+      </c>
+      <c r="P179">
+        <v>30</v>
+      </c>
+      <c r="T179" s="3">
+        <v>223703.4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>346</v>
+      </c>
+      <c r="B180" t="s">
+        <v>347</v>
+      </c>
+      <c r="C180" t="s">
+        <v>348</v>
+      </c>
+      <c r="D180" t="s">
+        <v>348</v>
+      </c>
+      <c r="P180">
+        <v>39</v>
+      </c>
+      <c r="T180" s="3">
+        <v>117297.42</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>322</v>
+      </c>
+      <c r="B181" t="s">
+        <v>323</v>
+      </c>
+      <c r="C181" t="s">
+        <v>324</v>
+      </c>
+      <c r="D181" t="s">
+        <v>324</v>
+      </c>
+      <c r="P181">
+        <v>37</v>
+      </c>
+      <c r="T181" s="3">
+        <v>89080.24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>306</v>
+      </c>
+      <c r="B182" t="s">
+        <v>307</v>
+      </c>
+      <c r="C182" t="s">
+        <v>308</v>
+      </c>
+      <c r="D182" t="s">
+        <v>308</v>
+      </c>
+      <c r="P182">
+        <v>33</v>
+      </c>
+      <c r="T182" s="3">
+        <v>69887.399999999994</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>298</v>
+      </c>
+      <c r="B183" t="s">
+        <v>299</v>
+      </c>
+      <c r="C183" t="s">
+        <v>300</v>
+      </c>
+      <c r="D183" t="s">
+        <v>300</v>
+      </c>
+      <c r="P183">
+        <v>21</v>
+      </c>
+      <c r="T183" s="3">
+        <v>65829.66</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>330</v>
+      </c>
+      <c r="B184" t="s">
+        <v>331</v>
+      </c>
+      <c r="C184" t="s">
+        <v>332</v>
+      </c>
+      <c r="D184" t="s">
+        <v>332</v>
+      </c>
+      <c r="P184">
+        <v>64</v>
+      </c>
+      <c r="T184" s="3">
+        <v>64488.05</v>
+      </c>
+    </row>
+    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>23</v>
+      </c>
+      <c r="B185" t="s">
+        <v>24</v>
+      </c>
+      <c r="C185" t="s">
+        <v>25</v>
+      </c>
+      <c r="D185" t="s">
+        <v>25</v>
+      </c>
+      <c r="P185">
+        <v>38</v>
+      </c>
+      <c r="T185" s="3">
+        <v>64374.54</v>
+      </c>
+    </row>
+    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>318</v>
+      </c>
+      <c r="B186" t="s">
+        <v>319</v>
+      </c>
+      <c r="C186" t="s">
+        <v>320</v>
+      </c>
+      <c r="D186" t="s">
+        <v>320</v>
+      </c>
+      <c r="P186">
+        <v>14</v>
+      </c>
+      <c r="T186" s="3">
+        <v>59310.16</v>
+      </c>
+    </row>
+    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>160</v>
+      </c>
+      <c r="B187" t="s">
+        <v>161</v>
+      </c>
+      <c r="C187" t="s">
+        <v>162</v>
+      </c>
+      <c r="D187" t="s">
+        <v>162</v>
+      </c>
+      <c r="P187">
+        <v>13</v>
+      </c>
+      <c r="T187" s="3">
+        <v>41853.4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>107</v>
+      </c>
+      <c r="B188" t="s">
+        <v>108</v>
+      </c>
+      <c r="C188" t="s">
+        <v>109</v>
+      </c>
+      <c r="D188" t="s">
+        <v>109</v>
+      </c>
+      <c r="P188">
+        <v>9</v>
+      </c>
+      <c r="T188" s="3">
+        <v>38124.58</v>
+      </c>
+    </row>
+    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>59</v>
+      </c>
+      <c r="B189" t="s">
+        <v>60</v>
+      </c>
+      <c r="C189" t="s">
+        <v>61</v>
+      </c>
+      <c r="D189" t="s">
+        <v>61</v>
+      </c>
+      <c r="P189">
+        <v>59</v>
+      </c>
+      <c r="T189" s="3">
+        <v>32450</v>
+      </c>
+    </row>
+    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>120</v>
+      </c>
+      <c r="B190" t="s">
+        <v>121</v>
+      </c>
+      <c r="C190" t="s">
+        <v>122</v>
+      </c>
+      <c r="D190" t="s">
+        <v>122</v>
+      </c>
+      <c r="P190">
+        <v>10</v>
+      </c>
+      <c r="T190" s="3">
+        <v>32194.94</v>
+      </c>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>334</v>
+      </c>
+      <c r="B191" t="s">
+        <v>335</v>
+      </c>
+      <c r="C191" t="s">
+        <v>336</v>
+      </c>
+      <c r="D191" t="s">
+        <v>336</v>
+      </c>
+      <c r="P191">
+        <v>7</v>
+      </c>
+      <c r="T191" s="3">
+        <v>28468.639999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>39</v>
+      </c>
+      <c r="B192" t="s">
+        <v>40</v>
+      </c>
+      <c r="C192" t="s">
+        <v>41</v>
+      </c>
+      <c r="D192" t="s">
+        <v>41</v>
+      </c>
+      <c r="P192">
+        <v>20</v>
+      </c>
+      <c r="T192" s="3">
+        <v>26254.26</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>91</v>
+      </c>
+      <c r="B193" t="s">
+        <v>92</v>
+      </c>
+      <c r="C193" t="s">
+        <v>93</v>
+      </c>
+      <c r="D193" t="s">
+        <v>93</v>
+      </c>
+      <c r="P193">
+        <v>19</v>
+      </c>
+      <c r="T193" s="3">
+        <v>24935.66</v>
+      </c>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>178</v>
+      </c>
+      <c r="B194" t="s">
+        <v>179</v>
+      </c>
+      <c r="C194" t="s">
+        <v>180</v>
+      </c>
+      <c r="D194" t="s">
+        <v>180</v>
+      </c>
+      <c r="P194">
+        <v>5</v>
+      </c>
+      <c r="T194" s="3">
+        <v>24572.03</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>140</v>
+      </c>
+      <c r="B195" t="s">
+        <v>141</v>
+      </c>
+      <c r="C195" t="s">
+        <v>142</v>
+      </c>
+      <c r="D195" t="s">
+        <v>142</v>
+      </c>
+      <c r="P195">
+        <v>7</v>
+      </c>
+      <c r="T195" s="3">
+        <v>23722.86</v>
+      </c>
+    </row>
+    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>358</v>
+      </c>
+      <c r="B196" t="s">
+        <v>359</v>
+      </c>
+      <c r="C196" t="s">
+        <v>360</v>
+      </c>
+      <c r="D196" t="s">
+        <v>360</v>
+      </c>
+      <c r="P196">
+        <v>8</v>
+      </c>
+      <c r="T196" s="3">
+        <v>23195.08</v>
+      </c>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>35</v>
+      </c>
+      <c r="B197" t="s">
+        <v>36</v>
+      </c>
+      <c r="C197" t="s">
+        <v>37</v>
+      </c>
+      <c r="D197" t="s">
+        <v>37</v>
+      </c>
+      <c r="P197">
+        <v>48</v>
+      </c>
+      <c r="T197" s="3">
+        <v>22332.14</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>326</v>
+      </c>
+      <c r="B198" t="s">
+        <v>327</v>
+      </c>
+      <c r="C198" t="s">
+        <v>328</v>
+      </c>
+      <c r="D198" t="s">
+        <v>328</v>
+      </c>
+      <c r="P198">
+        <v>17</v>
+      </c>
+      <c r="T198" s="3">
+        <v>22135.599999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>441</v>
+      </c>
+      <c r="B199" t="s">
+        <v>442</v>
+      </c>
+      <c r="C199" t="s">
+        <v>443</v>
+      </c>
+      <c r="D199" t="s">
+        <v>443</v>
+      </c>
+      <c r="P199">
+        <v>7</v>
+      </c>
+      <c r="T199" s="3">
+        <v>21350</v>
+      </c>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>144</v>
+      </c>
+      <c r="B200" t="s">
+        <v>145</v>
+      </c>
+      <c r="C200" t="s">
+        <v>146</v>
+      </c>
+      <c r="D200" t="s">
+        <v>146</v>
+      </c>
+      <c r="P200">
+        <v>9</v>
+      </c>
+      <c r="T200" s="3">
+        <v>17916.12</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>75</v>
+      </c>
+      <c r="B201" t="s">
+        <v>76</v>
+      </c>
+      <c r="C201" t="s">
+        <v>77</v>
+      </c>
+      <c r="D201" t="s">
+        <v>77</v>
+      </c>
+      <c r="P201">
+        <v>2</v>
+      </c>
+      <c r="T201" s="3">
+        <v>16947.46</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>234</v>
+      </c>
+      <c r="B202" t="s">
+        <v>235</v>
+      </c>
+      <c r="C202" t="s">
+        <v>236</v>
+      </c>
+      <c r="D202" t="s">
+        <v>236</v>
+      </c>
+      <c r="P202">
+        <v>5</v>
+      </c>
+      <c r="T202" s="3">
+        <v>16461.02</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>174</v>
+      </c>
+      <c r="B203" t="s">
+        <v>175</v>
+      </c>
+      <c r="C203" t="s">
+        <v>176</v>
+      </c>
+      <c r="D203" t="s">
+        <v>176</v>
+      </c>
+      <c r="P203">
+        <v>5</v>
+      </c>
+      <c r="T203" s="3">
+        <v>15018.64</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>170</v>
+      </c>
+      <c r="B204" t="s">
+        <v>171</v>
+      </c>
+      <c r="C204" t="s">
+        <v>172</v>
+      </c>
+      <c r="D204" t="s">
+        <v>172</v>
+      </c>
+      <c r="P204">
+        <v>5</v>
+      </c>
+      <c r="T204" s="3">
+        <v>14826.26</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>202</v>
+      </c>
+      <c r="B205" t="s">
+        <v>203</v>
+      </c>
+      <c r="C205" t="s">
+        <v>204</v>
+      </c>
+      <c r="D205" t="s">
+        <v>204</v>
+      </c>
+      <c r="P205">
+        <v>8</v>
+      </c>
+      <c r="T205" s="3">
+        <v>13552.54</v>
+      </c>
+    </row>
+    <row r="206" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>418</v>
+      </c>
+      <c r="B206" t="s">
+        <v>419</v>
+      </c>
+      <c r="C206" t="s">
+        <v>420</v>
+      </c>
+      <c r="D206" t="s">
+        <v>420</v>
+      </c>
+      <c r="P206">
+        <v>2</v>
+      </c>
+      <c r="T206" s="3">
+        <v>12478.97</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>87</v>
+      </c>
+      <c r="B207" t="s">
+        <v>88</v>
+      </c>
+      <c r="C207" t="s">
+        <v>89</v>
+      </c>
+      <c r="D207" t="s">
+        <v>89</v>
+      </c>
+      <c r="P207">
+        <v>9</v>
+      </c>
+      <c r="T207" s="3">
+        <v>11965.26</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>406</v>
+      </c>
+      <c r="B208" t="s">
+        <v>407</v>
+      </c>
+      <c r="C208" t="s">
+        <v>408</v>
+      </c>
+      <c r="D208" t="s">
+        <v>408</v>
+      </c>
+      <c r="P208">
+        <v>1</v>
+      </c>
+      <c r="T208" s="3">
+        <v>11778.81</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>286</v>
+      </c>
+      <c r="B209" t="s">
+        <v>287</v>
+      </c>
+      <c r="C209" t="s">
+        <v>288</v>
+      </c>
+      <c r="D209" t="s">
+        <v>288</v>
+      </c>
+      <c r="P209">
+        <v>8</v>
+      </c>
+      <c r="T209" s="3">
+        <v>11476.3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>194</v>
+      </c>
+      <c r="B210" t="s">
+        <v>195</v>
+      </c>
+      <c r="C210" t="s">
+        <v>196</v>
+      </c>
+      <c r="D210" t="s">
+        <v>196</v>
+      </c>
+      <c r="P210">
+        <v>1</v>
+      </c>
+      <c r="T210" s="3">
+        <v>11355.08</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>246</v>
+      </c>
+      <c r="B211" t="s">
+        <v>247</v>
+      </c>
+      <c r="C211" t="s">
+        <v>248</v>
+      </c>
+      <c r="D211" t="s">
+        <v>248</v>
+      </c>
+      <c r="P211">
+        <v>5</v>
+      </c>
+      <c r="T211" s="3">
+        <v>10589</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>453</v>
+      </c>
+      <c r="B212" t="s">
+        <v>454</v>
+      </c>
+      <c r="C212" t="s">
+        <v>455</v>
+      </c>
+      <c r="D212" t="s">
+        <v>455</v>
+      </c>
+      <c r="P212">
+        <v>1</v>
+      </c>
+      <c r="T212" s="3">
+        <v>9956.7800000000007</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>190</v>
+      </c>
+      <c r="B213" t="s">
+        <v>191</v>
+      </c>
+      <c r="C213" t="s">
+        <v>192</v>
+      </c>
+      <c r="D213" t="s">
+        <v>192</v>
+      </c>
+      <c r="P213">
+        <v>3</v>
+      </c>
+      <c r="T213" s="3">
+        <v>9912.7199999999993</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>242</v>
+      </c>
+      <c r="B214" t="s">
+        <v>243</v>
+      </c>
+      <c r="C214" t="s">
+        <v>244</v>
+      </c>
+      <c r="D214" t="s">
+        <v>244</v>
+      </c>
+      <c r="P214">
+        <v>5</v>
+      </c>
+      <c r="T214" s="3">
+        <v>9317.7999999999993</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>362</v>
+      </c>
+      <c r="B215" t="s">
+        <v>363</v>
+      </c>
+      <c r="C215" t="s">
+        <v>364</v>
+      </c>
+      <c r="D215" t="s">
+        <v>364</v>
+      </c>
+      <c r="P215">
+        <v>5</v>
+      </c>
+      <c r="T215" s="3">
+        <v>7849.16</v>
+      </c>
+    </row>
+    <row r="216" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>103</v>
+      </c>
+      <c r="B216" t="s">
+        <v>104</v>
+      </c>
+      <c r="C216" t="s">
+        <v>105</v>
+      </c>
+      <c r="D216" t="s">
+        <v>105</v>
+      </c>
+      <c r="P216">
+        <v>4</v>
+      </c>
+      <c r="T216" s="3">
+        <v>7650.48</v>
+      </c>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>63</v>
+      </c>
+      <c r="B217" t="s">
+        <v>64</v>
+      </c>
+      <c r="C217" t="s">
+        <v>65</v>
+      </c>
+      <c r="D217" t="s">
+        <v>65</v>
+      </c>
+      <c r="P217">
+        <v>16</v>
+      </c>
+      <c r="T217" s="3">
+        <v>7444.03</v>
+      </c>
+    </row>
+    <row r="218" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>430</v>
+      </c>
+      <c r="B218" t="s">
+        <v>431</v>
+      </c>
+      <c r="C218" t="s">
+        <v>432</v>
+      </c>
+      <c r="D218" t="s">
+        <v>432</v>
+      </c>
+      <c r="P218">
+        <v>2</v>
+      </c>
+      <c r="T218" s="3">
+        <v>7116.94</v>
+      </c>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>206</v>
+      </c>
+      <c r="B219" t="s">
+        <v>207</v>
+      </c>
+      <c r="C219" t="s">
+        <v>208</v>
+      </c>
+      <c r="D219" t="s">
+        <v>208</v>
+      </c>
+      <c r="P219">
+        <v>4</v>
+      </c>
+      <c r="T219" s="3">
+        <v>6776.27</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>510</v>
+      </c>
+      <c r="B220" t="s">
+        <v>511</v>
+      </c>
+      <c r="C220" t="s">
+        <v>512</v>
+      </c>
+      <c r="D220" t="s">
+        <v>512</v>
+      </c>
+      <c r="P220">
+        <v>1</v>
+      </c>
+      <c r="T220" s="3">
+        <v>5931.36</v>
+      </c>
+    </row>
+    <row r="221" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>310</v>
+      </c>
+      <c r="B221" t="s">
+        <v>311</v>
+      </c>
+      <c r="C221" t="s">
+        <v>312</v>
+      </c>
+      <c r="D221" t="s">
+        <v>312</v>
+      </c>
+      <c r="P221">
+        <v>2</v>
+      </c>
+      <c r="T221" s="3">
+        <v>5930.51</v>
+      </c>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>166</v>
+      </c>
+      <c r="B222" t="s">
+        <v>167</v>
+      </c>
+      <c r="C222" t="s">
+        <v>168</v>
+      </c>
+      <c r="D222" t="s">
+        <v>168</v>
+      </c>
+      <c r="P222">
+        <v>4</v>
+      </c>
+      <c r="T222" s="3">
+        <v>5780.58</v>
+      </c>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>111</v>
+      </c>
+      <c r="B223" t="s">
+        <v>72</v>
+      </c>
+      <c r="C223" t="s">
+        <v>112</v>
+      </c>
+      <c r="D223" t="s">
+        <v>112</v>
+      </c>
+      <c r="P223">
+        <v>5</v>
+      </c>
+      <c r="T223" s="3">
+        <v>5504.24</v>
+      </c>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>314</v>
+      </c>
+      <c r="B224" t="s">
+        <v>315</v>
+      </c>
+      <c r="C224" t="s">
+        <v>316</v>
+      </c>
+      <c r="D224" t="s">
+        <v>316</v>
+      </c>
+      <c r="P224">
+        <v>8</v>
+      </c>
+      <c r="T224" s="3">
+        <v>5416.96</v>
+      </c>
+    </row>
+    <row r="225" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>378</v>
+      </c>
+      <c r="B225" t="s">
+        <v>379</v>
+      </c>
+      <c r="C225" t="s">
+        <v>380</v>
+      </c>
+      <c r="D225" t="s">
+        <v>380</v>
+      </c>
+      <c r="P225">
+        <v>2</v>
+      </c>
+      <c r="T225" s="3">
+        <v>5083.0600000000004</v>
+      </c>
+    </row>
+    <row r="226" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>445</v>
+      </c>
+      <c r="B226" t="s">
+        <v>446</v>
+      </c>
+      <c r="C226" t="s">
+        <v>447</v>
+      </c>
+      <c r="D226" t="s">
+        <v>447</v>
+      </c>
+      <c r="P226">
+        <v>13</v>
+      </c>
+      <c r="T226" s="3">
+        <v>4946.58</v>
+      </c>
+    </row>
+    <row r="227" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>136</v>
+      </c>
+      <c r="B227" t="s">
+        <v>137</v>
+      </c>
+      <c r="C227" t="s">
+        <v>138</v>
+      </c>
+      <c r="D227" t="s">
+        <v>138</v>
+      </c>
+      <c r="P227">
+        <v>11</v>
+      </c>
+      <c r="T227" s="3">
+        <v>4299.99</v>
+      </c>
+    </row>
+    <row r="228" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228" t="s">
+        <v>231</v>
+      </c>
+      <c r="C228" t="s">
+        <v>232</v>
+      </c>
+      <c r="D228" t="s">
+        <v>232</v>
+      </c>
+      <c r="P228">
+        <v>1</v>
+      </c>
+      <c r="T228" s="3">
+        <v>4066.95</v>
+      </c>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>99</v>
+      </c>
+      <c r="B229" t="s">
+        <v>100</v>
+      </c>
+      <c r="C229" t="s">
+        <v>101</v>
+      </c>
+      <c r="D229" t="s">
+        <v>101</v>
+      </c>
+      <c r="P229">
+        <v>2</v>
+      </c>
+      <c r="T229" s="3">
+        <v>3642.37</v>
+      </c>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>124</v>
+      </c>
+      <c r="B230" t="s">
+        <v>125</v>
+      </c>
+      <c r="C230" t="s">
+        <v>126</v>
+      </c>
+      <c r="D230" t="s">
+        <v>126</v>
+      </c>
+      <c r="P230">
+        <v>2</v>
+      </c>
+      <c r="T230" s="3">
+        <v>3388.12</v>
+      </c>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>402</v>
+      </c>
+      <c r="B231" t="s">
+        <v>403</v>
+      </c>
+      <c r="C231" t="s">
+        <v>404</v>
+      </c>
+      <c r="D231" t="s">
+        <v>404</v>
+      </c>
+      <c r="P231">
+        <v>1</v>
+      </c>
+      <c r="T231" s="3">
+        <v>3345.13</v>
+      </c>
+    </row>
+    <row r="232" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>55</v>
+      </c>
+      <c r="B232" t="s">
+        <v>56</v>
+      </c>
+      <c r="C232" t="s">
+        <v>57</v>
+      </c>
+      <c r="D232" t="s">
+        <v>57</v>
+      </c>
+      <c r="P232">
+        <v>2</v>
+      </c>
+      <c r="T232" s="3">
+        <v>3336.44</v>
+      </c>
+    </row>
+    <row r="233" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>262</v>
+      </c>
+      <c r="B233" t="s">
+        <v>263</v>
+      </c>
+      <c r="C233" t="s">
+        <v>264</v>
+      </c>
+      <c r="D233" t="s">
+        <v>264</v>
+      </c>
+      <c r="P233">
+        <v>3</v>
+      </c>
+      <c r="T233" s="3">
+        <v>3202.55</v>
+      </c>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>302</v>
+      </c>
+      <c r="B234" t="s">
+        <v>303</v>
+      </c>
+      <c r="C234" t="s">
+        <v>304</v>
+      </c>
+      <c r="D234" t="s">
+        <v>304</v>
+      </c>
+      <c r="P234">
+        <v>5</v>
+      </c>
+      <c r="T234" s="3">
+        <v>3173.74</v>
+      </c>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>294</v>
+      </c>
+      <c r="B235" t="s">
+        <v>295</v>
+      </c>
+      <c r="C235" t="s">
+        <v>296</v>
+      </c>
+      <c r="D235" t="s">
+        <v>296</v>
+      </c>
+      <c r="P235">
+        <v>1</v>
+      </c>
+      <c r="T235" s="3">
+        <v>3134.75</v>
+      </c>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>132</v>
+      </c>
+      <c r="B236" t="s">
+        <v>133</v>
+      </c>
+      <c r="C236" t="s">
+        <v>134</v>
+      </c>
+      <c r="D236" t="s">
+        <v>134</v>
+      </c>
+      <c r="P236">
+        <v>4</v>
+      </c>
+      <c r="T236" s="3">
+        <v>2989.84</v>
+      </c>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>79</v>
+      </c>
+      <c r="B237" t="s">
+        <v>80</v>
+      </c>
+      <c r="C237" t="s">
+        <v>81</v>
+      </c>
+      <c r="D237" t="s">
+        <v>81</v>
+      </c>
+      <c r="P237">
+        <v>1</v>
+      </c>
+      <c r="T237" s="3">
+        <v>2820.34</v>
+      </c>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>374</v>
+      </c>
+      <c r="B238" t="s">
+        <v>375</v>
+      </c>
+      <c r="C238" t="s">
+        <v>376</v>
+      </c>
+      <c r="D238" t="s">
+        <v>376</v>
+      </c>
+      <c r="P238">
+        <v>1</v>
+      </c>
+      <c r="T238" s="3">
+        <v>2711.02</v>
+      </c>
+    </row>
+    <row r="239" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>116</v>
+      </c>
+      <c r="B239" t="s">
+        <v>117</v>
+      </c>
+      <c r="C239" t="s">
+        <v>118</v>
+      </c>
+      <c r="D239" t="s">
+        <v>118</v>
+      </c>
+      <c r="P239">
+        <v>2</v>
+      </c>
+      <c r="T239" s="3">
+        <v>2201.69</v>
+      </c>
+    </row>
+    <row r="240" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>290</v>
+      </c>
+      <c r="B240" t="s">
+        <v>291</v>
+      </c>
+      <c r="C240" t="s">
+        <v>292</v>
+      </c>
+      <c r="D240" t="s">
+        <v>292</v>
+      </c>
+      <c r="P240">
+        <v>1</v>
+      </c>
+      <c r="T240" s="3">
+        <v>2117.8000000000002</v>
+      </c>
+    </row>
+    <row r="241" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>270</v>
+      </c>
+      <c r="B241" t="s">
+        <v>271</v>
+      </c>
+      <c r="C241" t="s">
+        <v>272</v>
+      </c>
+      <c r="D241" t="s">
+        <v>272</v>
+      </c>
+      <c r="P241">
+        <v>1</v>
+      </c>
+      <c r="T241" s="3">
+        <v>1821.19</v>
+      </c>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>438</v>
+      </c>
+      <c r="B242" t="s">
+        <v>215</v>
+      </c>
+      <c r="C242" t="s">
+        <v>439</v>
+      </c>
+      <c r="D242" t="s">
+        <v>439</v>
+      </c>
+      <c r="P242">
+        <v>1</v>
+      </c>
+      <c r="T242" s="3">
+        <v>1694.07</v>
+      </c>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>254</v>
+      </c>
+      <c r="B243" t="s">
+        <v>255</v>
+      </c>
+      <c r="C243" t="s">
+        <v>256</v>
+      </c>
+      <c r="D243" t="s">
+        <v>256</v>
+      </c>
+      <c r="P243">
+        <v>1</v>
+      </c>
+      <c r="T243" s="3">
+        <v>1143.22</v>
+      </c>
+    </row>
+    <row r="244" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>338</v>
+      </c>
+      <c r="B244" t="s">
+        <v>339</v>
+      </c>
+      <c r="C244" t="s">
+        <v>340</v>
+      </c>
+      <c r="D244" t="s">
+        <v>340</v>
+      </c>
+      <c r="P244">
+        <v>1</v>
+      </c>
+      <c r="T244" s="3">
+        <v>1143.22</v>
+      </c>
+    </row>
+    <row r="245" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>250</v>
+      </c>
+      <c r="B245" t="s">
+        <v>251</v>
+      </c>
+      <c r="C245" t="s">
+        <v>252</v>
+      </c>
+      <c r="D245" t="s">
+        <v>252</v>
+      </c>
+      <c r="P245">
+        <v>0</v>
+      </c>
+      <c r="T245" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>394</v>
+      </c>
+      <c r="B246" t="s">
+        <v>395</v>
+      </c>
+      <c r="C246" t="s">
+        <v>396</v>
+      </c>
+      <c r="D246" t="s">
+        <v>396</v>
+      </c>
+      <c r="P246">
+        <v>0</v>
+      </c>
+      <c r="T246" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>164</v>
+      </c>
+      <c r="B247" t="s">
+        <v>28</v>
+      </c>
+      <c r="C247" t="s">
+        <v>165</v>
+      </c>
+      <c r="D247" t="s">
+        <v>165</v>
+      </c>
+      <c r="P247">
+        <v>0</v>
+      </c>
+      <c r="T247" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>186</v>
+      </c>
+      <c r="B248" t="s">
+        <v>187</v>
+      </c>
+      <c r="C248" t="s">
+        <v>188</v>
+      </c>
+      <c r="D248" t="s">
+        <v>188</v>
+      </c>
+      <c r="P248">
+        <v>0</v>
+      </c>
+      <c r="T248" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>182</v>
+      </c>
+      <c r="B249" t="s">
+        <v>183</v>
+      </c>
+      <c r="C249" t="s">
+        <v>184</v>
+      </c>
+      <c r="D249" t="s">
+        <v>184</v>
+      </c>
+      <c r="P249">
+        <v>0</v>
+      </c>
+      <c r="T249" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>354</v>
+      </c>
+      <c r="B250" t="s">
+        <v>355</v>
+      </c>
+      <c r="C250" t="s">
+        <v>356</v>
+      </c>
+      <c r="D250" t="s">
+        <v>356</v>
+      </c>
+      <c r="P250">
+        <v>0</v>
+      </c>
+      <c r="T250" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>390</v>
+      </c>
+      <c r="B251" t="s">
+        <v>391</v>
+      </c>
+      <c r="C251" t="s">
+        <v>392</v>
+      </c>
+      <c r="D251" t="s">
+        <v>392</v>
+      </c>
+      <c r="P251">
+        <v>0</v>
+      </c>
+      <c r="T251" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>